<commit_message>
Thông Kê Trạng Thái Và Fix Nhân Viên
</commit_message>
<xml_diff>
--- a/public/EmployeeTemplate.xlsx
+++ b/public/EmployeeTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\DATN\Code\FE_DATN\du-an-ban-ao-nam\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FPT Polytechnic\DATN\Code\FE_DATN\DATN-FE\du-an-ban-ao-nam\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32F0AF95-4C21-44A5-8D48-082480B7932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15436D55-24F9-4F70-80C3-DDED5663310D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="468" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NhanVien" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Tên Nhân Viên</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Ghi Chú</t>
   </si>
   <si>
-    <t>Vai Trò</t>
-  </si>
-  <si>
-    <t>Trạng Thái</t>
-  </si>
-  <si>
     <t>Nam</t>
   </si>
   <si>
@@ -70,9 +64,6 @@
     <t/>
   </si>
   <si>
-    <t>Nhân viên</t>
-  </si>
-  <si>
     <t>0213213213</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
   </si>
   <si>
     <t>Xã Bình Định</t>
-  </si>
-  <si>
-    <t>Đang hoạt động</t>
   </si>
   <si>
     <t>sadsa</t>
@@ -478,7 +466,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,51 +520,41 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
       <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>